<commit_message>
Update format. Create pdf files
</commit_message>
<xml_diff>
--- a/Guideline/Sakai/Guideline_Deploy-elearning-portal-with-Sakai_Basic.xlsx
+++ b/Guideline/Sakai/Guideline_Deploy-elearning-portal-with-Sakai_Basic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="11340" windowHeight="8535" tabRatio="991" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="11340" windowHeight="8535" tabRatio="991" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="9" r:id="rId1"/>
@@ -7413,6 +7413,10 @@
   </sheetData>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;LHow to use sakai</oddHeader>
+    <oddFooter>&amp;R&amp;P/&amp;N</oddFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -7421,7 +7425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H473"/>
   <sheetViews>
-    <sheetView topLeftCell="A348" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AB481" sqref="AB481"/>
     </sheetView>
   </sheetViews>
@@ -7551,6 +7555,10 @@
   </sheetData>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;LHow to use sakai</oddHeader>
+    <oddFooter>&amp;R&amp;P/&amp;N</oddFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -16394,7 +16402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AR221" sqref="AR221"/>
     </sheetView>
   </sheetViews>
@@ -16668,6 +16676,7 @@
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
+    <oddHeader>&amp;LHow to use Sakai</oddHeader>
     <oddFooter>&amp;L&amp;"Symbol,Regular"Ó &amp;"Arial,Regular"Thach N. Le&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
@@ -16678,7 +16687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A241" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -16775,6 +16784,7 @@
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
+    <oddHeader>&amp;LHow to use Sakai</oddHeader>
     <oddFooter>&amp;L&amp;"Symbol,Regular"Ó &amp;"Arial,Regular"Thach N. Le&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>

</xml_diff>